<commit_message>
Updates the sample Excel file
Updated the `shopee_sample.xlsx` file with new sample data.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: e3eb3c96-df70-4906-879e-aee18a3268c0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/febc32d6-9ae9-48e6-a5ba-59519be0a0c9/4a967625-8cff-4363-9097-1b976a5c917c.jpg
</commit_message>
<xml_diff>
--- a/shopee_sample.xlsx
+++ b/shopee_sample.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,6 +27,9 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <color rgb="00AA0000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,12 +480,6 @@
           <t>link_column=A;var1_column=B;var2_column=C;discount_column=D</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr"/>
-      <c r="D2" t="inlineStr"/>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -499,8 +497,6 @@
           <t>128GB</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>27500000</v>
       </c>
@@ -524,8 +520,9 @@
           <t>256GB</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr"/>
-      <c r="E4" t="inlineStr"/>
+      <c r="D4" s="2" t="n">
+        <v>-0.2320185614849146</v>
+      </c>
       <c r="F4" t="n">
         <v>21500000</v>
       </c>
@@ -539,10 +536,9 @@
           <t>https://shopee.vn/Tai-nghe-Apple-AirPods-Pro-2-2022-i.88201679.11893691238</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr"/>
-      <c r="D5" t="inlineStr"/>
-      <c r="E5" t="inlineStr"/>
+      <c r="D5" s="2" t="n">
+        <v>-0.08936550491509543</v>
+      </c>
       <c r="F5" t="n">
         <v>5590000</v>
       </c>
@@ -566,8 +562,9 @@
           <t>64GB</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
+      <c r="D6" s="2" t="n">
+        <v>-0.540540540540535</v>
+      </c>
       <c r="F6" t="n">
         <v>9200000</v>
       </c>
@@ -591,8 +588,9 @@
           <t>41mm</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr"/>
-      <c r="E7" t="inlineStr"/>
+      <c r="D7" s="2" t="n">
+        <v>-0.4739336492890933</v>
+      </c>
       <c r="F7" t="n">
         <v>10500000</v>
       </c>

</xml_diff>

<commit_message>
Added sample data and deployment instructions
Added a sample Excel file, README with local and Render deployment instructions, and configured the project for deployment on Render.  Files modified include `create_sample_excel.py`, `shopee_sample.xlsx`, `.gitignore`, `Procfile`, `README.md`, `render.yaml`, and `requirements.txt.sample`.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: e3eb3c96-df70-4906-879e-aee18a3268c0
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/febc32d6-9ae9-48e6-a5ba-59519be0a0c9/5b3b319e-dccf-447b-9c6e-024f6b867e48.jpg
</commit_message>
<xml_diff>
--- a/shopee_sample.xlsx
+++ b/shopee_sample.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,9 +27,6 @@
     </font>
     <font>
       <b val="1"/>
-    </font>
-    <font>
-      <color rgb="00AA0000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -58,12 +55,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -429,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,6 +476,12 @@
           <t>link_column=A;var1_column=B;var2_column=C;discount_column=D</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -497,6 +499,8 @@
           <t>128GB</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
       <c r="F3" t="n">
         <v>27500000</v>
       </c>
@@ -520,9 +524,8 @@
           <t>256GB</t>
         </is>
       </c>
-      <c r="D4" s="2" t="n">
-        <v>-0.2320185614849146</v>
-      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
       <c r="F4" t="n">
         <v>21500000</v>
       </c>
@@ -536,9 +539,10 @@
           <t>https://shopee.vn/Tai-nghe-Apple-AirPods-Pro-2-2022-i.88201679.11893691238</t>
         </is>
       </c>
-      <c r="D5" s="2" t="n">
-        <v>-0.08936550491509543</v>
-      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
+      <c r="E5" t="inlineStr"/>
       <c r="F5" t="n">
         <v>5590000</v>
       </c>
@@ -562,9 +566,8 @@
           <t>64GB</t>
         </is>
       </c>
-      <c r="D6" s="2" t="n">
-        <v>-0.540540540540535</v>
-      </c>
+      <c r="D6" t="inlineStr"/>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="n">
         <v>9200000</v>
       </c>
@@ -588,14 +591,101 @@
           <t>41mm</t>
         </is>
       </c>
-      <c r="D7" s="2" t="n">
-        <v>-0.4739336492890933</v>
-      </c>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
       <c r="F7" t="n">
         <v>10500000</v>
       </c>
       <c r="G7" t="n">
         <v>10600000</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>https://shopee.vn/Samsung-Galaxy-S24-Ultra-12GB-256GB-i.88201679.23626487486</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Đen</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>256GB</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr"/>
+      <c r="E8" t="inlineStr"/>
+      <c r="F8" t="n">
+        <v>28990000</v>
+      </c>
+      <c r="G8" t="n">
+        <v>29500000</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>https://shopee.vn/Google-Pixel-8-Pro-128GB-Ch%C3%ADnh-H%C3%A3ng-i.88201679.23548769421</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Xanh</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>128GB</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr"/>
+      <c r="E9" t="inlineStr"/>
+      <c r="F9" t="n">
+        <v>21490000</v>
+      </c>
+      <c r="G9" t="n">
+        <v>21990000</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>https://shopee.vn/Laptop-Dell-XPS-13-Plus-9320-i7-1260P-16GB-512GB-Windows-11-i.88201679.21845126497</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>512GB</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr"/>
+      <c r="E10" t="inlineStr"/>
+      <c r="F10" t="n">
+        <v>38990000</v>
+      </c>
+      <c r="G10" t="n">
+        <v>39900000</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>https://shopee.vn/Laptop-Gaming-Asus-ROG-Strix-G16-G614JV-N4086W-i7-13650HX-16GB-512GB-RTX-4060-Windows-11-i.88201679.22274851269</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
+      <c r="E11" t="inlineStr"/>
+      <c r="F11" t="n">
+        <v>39490000</v>
+      </c>
+      <c r="G11" t="n">
+        <v>39990000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>